<commit_message>
Updated the Acceptance Test Plan spreadsheet.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kennm\Documents\RIT\u-fund\U_FUND-SEED-REPO\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmt4444\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DBA5D3-C5F2-43B0-9D5A-B4A8B876B0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8065964-04D6-4FE1-9F6C-A647F17C0F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6645" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Instructions</t>
   </si>
@@ -544,6 +544,216 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>DT ; 11/13/23 ; After login, you can see the Needs, but there is no specific 'Needs' page</t>
+  </si>
+  <si>
+    <t>DT ; 11/13/23 ;</t>
+  </si>
+  <si>
+    <t>DT; 11/13/23 ;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Developer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I want to Submit a request to get a need from the need cupboard so that it is added to the funding basket.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I am a developer when submit a request to the rest api server then I am able to add a need from the needs cupboard to the funding basket. </t>
+  </si>
+  <si>
+    <t>DT ; 11/12/23 ;</t>
+  </si>
+  <si>
+    <t>Given I am a developer when I try to create a need that is not also in the need cupboard then I get a 404 not found error.</t>
+  </si>
+  <si>
+    <t>Given I am a developer when I try to create a need that already exists then I get a 409 conflict error.</t>
+  </si>
+  <si>
+    <t>Given I am a developer when submit a get request to the server then I should receive the needs in the funding basket.</t>
+  </si>
+  <si>
+    <t>Given I am a developer when I submit a request to delete a need in the funding basket then the need will be deleted.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Developer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I want to Submit a request to get the funding basket so that I can view all the needs in the funding basket.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Developer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I want to Submit a request to delete a need so that it is no longer in the funding basket.</t>
+    </r>
+  </si>
+  <si>
+    <t>Given I am an admin when I log in then I EXPECT to be able to add/delete/edit needs from the cupboard.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>manager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I want to log in so that I can manage the needs cupboard.</t>
+    </r>
+  </si>
+  <si>
+    <t>Given there is a search bar on screen when I type in a characters then I expect needs to come up below the bar.</t>
+  </si>
+  <si>
+    <t>Given there is a search bar on screen when I type in a characters then I expect matching needs to pop up below.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>manager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I want to add to, remove from, and edit the needs cupboard so that the helpers can order the correct needs.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>helper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I want to search for a specific need so that I can narrow down the needs that I want to fund.</t>
+    </r>
+  </si>
+  <si>
+    <t>Given I am an admin when I click add Need a need to the database then I am able to add a need from the needs cupboard</t>
+  </si>
+  <si>
+    <t>Given I am an admin when I click add the 'X' icon then I am able to delete a Need from the need cupboard.</t>
+  </si>
+  <si>
+    <t>Given I am an admin when I click a need and edit its details then I am able to update that need within the need cupboard</t>
+  </si>
+  <si>
+    <t>SPRINT 3 STUFF:</t>
+  </si>
+  <si>
+    <t>None ready for testing yet.</t>
   </si>
 </sst>
 </file>
@@ -608,7 +818,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -625,11 +835,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -660,6 +899,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,7 +1338,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1128,7 +1379,12 @@
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1152,7 +1408,12 @@
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1160,112 +1421,220 @@
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="8"/>
+    <row r="7" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="8"/>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="8"/>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="8"/>
+    <row r="14" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="8"/>
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="8"/>
+    <row r="16" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="8"/>
+    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="8"/>
+    <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="14"/>
       <c r="C19" s="8"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C20" s="8"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="8"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" s="8"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" s="8"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="8"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="8"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" s="8"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" s="8"/>
       <c r="E32" s="8"/>
     </row>
@@ -3499,7 +3868,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D587 F2:F587">
+  <conditionalFormatting sqref="F2:F587 D2:D587">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -3513,7 +3882,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>